<commit_message>
consider left and right in calculation
</commit_message>
<xml_diff>
--- a/word gen/wordlist.xlsx
+++ b/word gen/wordlist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UserPC\Documents\Dyslexia\word gen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\POOM\Desktop\Dyslexia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93513097-5AE4-40A5-B952-DC2752C44925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2418E862-C4A2-4668-A9AD-B2A0047FD945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-210" yWindow="2145" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11748" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="397">
   <si>
     <t>image id</t>
   </si>
@@ -931,9 +931,6 @@
     <t>cod</t>
   </si>
   <si>
-    <t>ceq</t>
-  </si>
-  <si>
     <t>eor</t>
   </si>
   <si>
@@ -1012,7 +1009,208 @@
     <t>knan</t>
   </si>
   <si>
-    <t>nona</t>
+    <t>nuna</t>
+  </si>
+  <si>
+    <t>lech</t>
+  </si>
+  <si>
+    <t>lach</t>
+  </si>
+  <si>
+    <t>dult</t>
+  </si>
+  <si>
+    <t>rora</t>
+  </si>
+  <si>
+    <t>hanu</t>
+  </si>
+  <si>
+    <t>juap</t>
+  </si>
+  <si>
+    <t>gary</t>
+  </si>
+  <si>
+    <t>knus</t>
+  </si>
+  <si>
+    <t>druto</t>
+  </si>
+  <si>
+    <t>biwol</t>
+  </si>
+  <si>
+    <t>maron</t>
+  </si>
+  <si>
+    <t>awlas</t>
+  </si>
+  <si>
+    <t>tonat</t>
+  </si>
+  <si>
+    <t>cep</t>
+  </si>
+  <si>
+    <t>dorat</t>
+  </si>
+  <si>
+    <t>wlnad</t>
+  </si>
+  <si>
+    <t>lenam</t>
+  </si>
+  <si>
+    <t>racie</t>
+  </si>
+  <si>
+    <t>denog</t>
+  </si>
+  <si>
+    <t>cowok</t>
+  </si>
+  <si>
+    <t>sveck</t>
+  </si>
+  <si>
+    <t>carno</t>
+  </si>
+  <si>
+    <t>slary</t>
+  </si>
+  <si>
+    <t>aronu</t>
+  </si>
+  <si>
+    <t>ralie</t>
+  </si>
+  <si>
+    <t>plisk</t>
+  </si>
+  <si>
+    <t>tenal</t>
+  </si>
+  <si>
+    <t>sysna</t>
+  </si>
+  <si>
+    <t>zabon</t>
+  </si>
+  <si>
+    <t>strufa</t>
+  </si>
+  <si>
+    <t>wichyn</t>
+  </si>
+  <si>
+    <t>pilder</t>
+  </si>
+  <si>
+    <t>ardana</t>
+  </si>
+  <si>
+    <t>trypez</t>
+  </si>
+  <si>
+    <t>eczera</t>
+  </si>
+  <si>
+    <t>rudnik</t>
+  </si>
+  <si>
+    <t>slaimy</t>
+  </si>
+  <si>
+    <t>bectka</t>
+  </si>
+  <si>
+    <t>syspem</t>
+  </si>
+  <si>
+    <t>czalka</t>
+  </si>
+  <si>
+    <t>krodka</t>
+  </si>
+  <si>
+    <t>ponout</t>
+  </si>
+  <si>
+    <t>jeyura</t>
+  </si>
+  <si>
+    <t>sfepto</t>
+  </si>
+  <si>
+    <t>trepel</t>
+  </si>
+  <si>
+    <t>becaro</t>
+  </si>
+  <si>
+    <t>pipumr</t>
+  </si>
+  <si>
+    <t>luplip</t>
+  </si>
+  <si>
+    <t>sorpekt</t>
+  </si>
+  <si>
+    <t>glianca</t>
+  </si>
+  <si>
+    <t>bolkarg</t>
+  </si>
+  <si>
+    <t>silpare</t>
+  </si>
+  <si>
+    <t>sefitis</t>
+  </si>
+  <si>
+    <t>gatolka</t>
+  </si>
+  <si>
+    <t>posocyt</t>
+  </si>
+  <si>
+    <t>podlana</t>
+  </si>
+  <si>
+    <t>squratz</t>
+  </si>
+  <si>
+    <t>sounern</t>
+  </si>
+  <si>
+    <t>nesttol</t>
+  </si>
+  <si>
+    <t>beczika</t>
+  </si>
+  <si>
+    <t>vandere</t>
+  </si>
+  <si>
+    <t>sqeolae</t>
+  </si>
+  <si>
+    <t>rusarin</t>
+  </si>
+  <si>
+    <t>prasker</t>
+  </si>
+  <si>
+    <t>owlawki</t>
+  </si>
+  <si>
+    <t>samosus</t>
+  </si>
+  <si>
+    <t>tiblect</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1257,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1361,13 +1559,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1375,16 +1573,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1392,16 +1590,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1409,16 +1607,16 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1426,16 +1624,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1443,16 +1641,16 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1460,16 +1658,16 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1477,16 +1675,16 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
+        <v>304</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1494,16 +1692,16 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1511,16 +1709,16 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
+        <v>306</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1528,16 +1726,16 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
+        <v>307</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1545,16 +1743,16 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
+        <v>308</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1562,16 +1760,16 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
+        <v>309</v>
+      </c>
+      <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>35</v>
       </c>
-      <c r="E12" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1579,16 +1777,16 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>38</v>
       </c>
-      <c r="E13" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1596,16 +1794,16 @@
         <v>39</v>
       </c>
       <c r="C14" t="s">
+        <v>311</v>
+      </c>
+      <c r="D14" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>41</v>
       </c>
-      <c r="E14" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1613,16 +1811,16 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
+        <v>312</v>
+      </c>
+      <c r="D15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1630,16 +1828,16 @@
         <v>45</v>
       </c>
       <c r="C16" t="s">
+        <v>313</v>
+      </c>
+      <c r="D16" t="s">
         <v>46</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="E16" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1647,16 +1845,16 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
+        <v>314</v>
+      </c>
+      <c r="D17" t="s">
         <v>48</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>49</v>
       </c>
-      <c r="E17" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1664,16 +1862,16 @@
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>316</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
+        <v>315</v>
+      </c>
+      <c r="E18" t="s">
         <v>51</v>
       </c>
-      <c r="E18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1681,16 +1879,16 @@
         <v>52</v>
       </c>
       <c r="C19" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>54</v>
       </c>
-      <c r="E19" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1698,16 +1896,16 @@
         <v>55</v>
       </c>
       <c r="C20" t="s">
+        <v>317</v>
+      </c>
+      <c r="D20" t="s">
         <v>56</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>57</v>
       </c>
-      <c r="E20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1715,67 +1913,67 @@
         <v>58</v>
       </c>
       <c r="C21" t="s">
+        <v>318</v>
+      </c>
+      <c r="D21" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>60</v>
       </c>
-      <c r="E21" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D22" t="s">
         <v>62</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D23" t="s">
         <v>65</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D24" t="s">
         <v>68</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1783,33 +1981,33 @@
         <v>70</v>
       </c>
       <c r="C25" t="s">
+        <v>322</v>
+      </c>
+      <c r="D25" t="s">
         <v>71</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>72</v>
       </c>
-      <c r="E25" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D26" t="s">
         <v>74</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1817,33 +2015,33 @@
         <v>76</v>
       </c>
       <c r="C27" t="s">
+        <v>324</v>
+      </c>
+      <c r="D27" t="s">
         <v>77</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>78</v>
       </c>
-      <c r="E27" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>79</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D28" t="s">
         <v>80</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1851,16 +2049,16 @@
         <v>82</v>
       </c>
       <c r="C29" t="s">
+        <v>326</v>
+      </c>
+      <c r="D29" t="s">
         <v>83</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>84</v>
       </c>
-      <c r="E29" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1868,50 +2066,50 @@
         <v>85</v>
       </c>
       <c r="C30" t="s">
+        <v>327</v>
+      </c>
+      <c r="D30" t="s">
         <v>86</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>87</v>
       </c>
-      <c r="E30" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>88</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D31" t="s">
         <v>89</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>91</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D32" t="s">
         <v>92</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>93</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1919,50 +2117,50 @@
         <v>94</v>
       </c>
       <c r="C33" t="s">
+        <v>329</v>
+      </c>
+      <c r="D33" t="s">
         <v>95</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="E33" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>97</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D34" t="s">
         <v>98</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>99</v>
       </c>
-      <c r="E34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>100</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D35" t="s">
         <v>101</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>102</v>
       </c>
-      <c r="E35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1970,33 +2168,33 @@
         <v>103</v>
       </c>
       <c r="C36" t="s">
+        <v>332</v>
+      </c>
+      <c r="D36" t="s">
         <v>104</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>105</v>
       </c>
-      <c r="E36" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>106</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D37" t="s">
         <v>107</v>
-      </c>
-      <c r="D37" t="s">
-        <v>106</v>
       </c>
       <c r="E37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2004,16 +2202,16 @@
         <v>108</v>
       </c>
       <c r="C38" t="s">
+        <v>334</v>
+      </c>
+      <c r="D38" t="s">
         <v>109</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>110</v>
       </c>
-      <c r="E38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2021,16 +2219,16 @@
         <v>111</v>
       </c>
       <c r="C39" t="s">
+        <v>335</v>
+      </c>
+      <c r="D39" t="s">
         <v>112</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>113</v>
       </c>
-      <c r="E39" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2038,16 +2236,16 @@
         <v>114</v>
       </c>
       <c r="C40" t="s">
+        <v>336</v>
+      </c>
+      <c r="D40" t="s">
         <v>115</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>116</v>
       </c>
-      <c r="E40" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2055,16 +2253,16 @@
         <v>117</v>
       </c>
       <c r="C41" t="s">
+        <v>337</v>
+      </c>
+      <c r="D41" t="s">
         <v>118</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>119</v>
       </c>
-      <c r="E41" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2072,16 +2270,16 @@
         <v>120</v>
       </c>
       <c r="C42" t="s">
+        <v>338</v>
+      </c>
+      <c r="D42" t="s">
         <v>121</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>122</v>
       </c>
-      <c r="E42" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2089,16 +2287,16 @@
         <v>123</v>
       </c>
       <c r="C43" t="s">
+        <v>339</v>
+      </c>
+      <c r="D43" t="s">
         <v>124</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>125</v>
       </c>
-      <c r="E43" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2106,16 +2304,16 @@
         <v>126</v>
       </c>
       <c r="C44" t="s">
+        <v>340</v>
+      </c>
+      <c r="D44" t="s">
         <v>127</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>128</v>
       </c>
-      <c r="E44" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2123,16 +2321,16 @@
         <v>129</v>
       </c>
       <c r="C45" t="s">
+        <v>341</v>
+      </c>
+      <c r="D45" t="s">
         <v>130</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>131</v>
       </c>
-      <c r="E45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2140,16 +2338,16 @@
         <v>132</v>
       </c>
       <c r="C46" t="s">
+        <v>342</v>
+      </c>
+      <c r="D46" t="s">
         <v>133</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>134</v>
       </c>
-      <c r="E46" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2157,16 +2355,16 @@
         <v>135</v>
       </c>
       <c r="C47" t="s">
+        <v>344</v>
+      </c>
+      <c r="D47" t="s">
         <v>136</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>137</v>
       </c>
-      <c r="E47" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2174,16 +2372,16 @@
         <v>138</v>
       </c>
       <c r="C48" t="s">
+        <v>345</v>
+      </c>
+      <c r="D48" t="s">
         <v>139</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>140</v>
       </c>
-      <c r="E48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2191,16 +2389,16 @@
         <v>141</v>
       </c>
       <c r="C49" t="s">
+        <v>346</v>
+      </c>
+      <c r="D49" t="s">
         <v>142</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>143</v>
       </c>
-      <c r="E49" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2208,16 +2406,16 @@
         <v>144</v>
       </c>
       <c r="C50" t="s">
+        <v>347</v>
+      </c>
+      <c r="D50" t="s">
         <v>145</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>146</v>
       </c>
-      <c r="E50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2225,16 +2423,16 @@
         <v>147</v>
       </c>
       <c r="C51" t="s">
+        <v>348</v>
+      </c>
+      <c r="D51" t="s">
         <v>148</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>149</v>
       </c>
-      <c r="E51" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2242,16 +2440,16 @@
         <v>150</v>
       </c>
       <c r="C52" t="s">
+        <v>349</v>
+      </c>
+      <c r="D52" t="s">
         <v>151</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>152</v>
       </c>
-      <c r="E52" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2259,16 +2457,16 @@
         <v>153</v>
       </c>
       <c r="C53" t="s">
+        <v>353</v>
+      </c>
+      <c r="D53" t="s">
         <v>154</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>155</v>
       </c>
-      <c r="E53" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2276,16 +2474,16 @@
         <v>156</v>
       </c>
       <c r="C54" t="s">
+        <v>350</v>
+      </c>
+      <c r="D54" t="s">
         <v>157</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>158</v>
       </c>
-      <c r="E54" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2293,16 +2491,16 @@
         <v>159</v>
       </c>
       <c r="C55" t="s">
+        <v>351</v>
+      </c>
+      <c r="D55" t="s">
         <v>160</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>161</v>
       </c>
-      <c r="E55" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2310,16 +2508,16 @@
         <v>162</v>
       </c>
       <c r="C56" t="s">
+        <v>352</v>
+      </c>
+      <c r="D56" t="s">
         <v>163</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>164</v>
       </c>
-      <c r="E56" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2327,33 +2525,33 @@
         <v>165</v>
       </c>
       <c r="C57" t="s">
+        <v>354</v>
+      </c>
+      <c r="D57" t="s">
         <v>166</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>167</v>
       </c>
-      <c r="E57" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>168</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D58" t="s">
         <v>169</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>170</v>
       </c>
-      <c r="E58" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2361,33 +2559,33 @@
         <v>171</v>
       </c>
       <c r="C59" t="s">
+        <v>356</v>
+      </c>
+      <c r="D59" t="s">
         <v>172</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>173</v>
       </c>
-      <c r="E59" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>174</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D60" t="s">
         <v>175</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>176</v>
       </c>
-      <c r="E60" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2395,16 +2593,16 @@
         <v>177</v>
       </c>
       <c r="C61" t="s">
+        <v>358</v>
+      </c>
+      <c r="D61" t="s">
         <v>178</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>179</v>
       </c>
-      <c r="E61" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2412,16 +2610,16 @@
         <v>180</v>
       </c>
       <c r="C62" t="s">
+        <v>359</v>
+      </c>
+      <c r="D62" t="s">
         <v>181</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>182</v>
       </c>
-      <c r="E62" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2429,16 +2627,16 @@
         <v>183</v>
       </c>
       <c r="C63" t="s">
+        <v>360</v>
+      </c>
+      <c r="D63" t="s">
         <v>184</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>185</v>
       </c>
-      <c r="E63" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2446,16 +2644,16 @@
         <v>186</v>
       </c>
       <c r="C64" t="s">
+        <v>361</v>
+      </c>
+      <c r="D64" t="s">
         <v>187</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>188</v>
       </c>
-      <c r="E64" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2463,16 +2661,16 @@
         <v>189</v>
       </c>
       <c r="C65" t="s">
+        <v>362</v>
+      </c>
+      <c r="D65" t="s">
         <v>190</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>191</v>
       </c>
-      <c r="E65" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2480,16 +2678,16 @@
         <v>192</v>
       </c>
       <c r="C66" t="s">
+        <v>363</v>
+      </c>
+      <c r="D66" t="s">
         <v>193</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>194</v>
       </c>
-      <c r="E66" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2497,16 +2695,16 @@
         <v>195</v>
       </c>
       <c r="C67" t="s">
+        <v>364</v>
+      </c>
+      <c r="D67" t="s">
         <v>196</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>197</v>
       </c>
-      <c r="E67" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2514,16 +2712,16 @@
         <v>198</v>
       </c>
       <c r="C68" t="s">
+        <v>365</v>
+      </c>
+      <c r="D68" t="s">
         <v>199</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>200</v>
       </c>
-      <c r="E68" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2531,101 +2729,101 @@
         <v>201</v>
       </c>
       <c r="C69" t="s">
+        <v>366</v>
+      </c>
+      <c r="D69" t="s">
         <v>202</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>203</v>
       </c>
-      <c r="E69" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>204</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D70" t="s">
         <v>205</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>206</v>
       </c>
-      <c r="E70" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>207</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D71" t="s">
         <v>208</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>209</v>
       </c>
-      <c r="E71" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>210</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D72" t="s">
         <v>211</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>212</v>
       </c>
-      <c r="E72" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>213</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D73" t="s">
         <v>214</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>215</v>
       </c>
-      <c r="E73" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>216</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D74" t="s">
         <v>217</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>218</v>
       </c>
-      <c r="E74" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2633,16 +2831,16 @@
         <v>219</v>
       </c>
       <c r="C75" t="s">
+        <v>372</v>
+      </c>
+      <c r="D75" t="s">
         <v>220</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>221</v>
       </c>
-      <c r="E75" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2650,33 +2848,33 @@
         <v>222</v>
       </c>
       <c r="C76" t="s">
+        <v>373</v>
+      </c>
+      <c r="D76" t="s">
         <v>223</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>224</v>
       </c>
-      <c r="E76" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>225</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D77" t="s">
         <v>226</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>227</v>
       </c>
-      <c r="E77" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2684,16 +2882,16 @@
         <v>228</v>
       </c>
       <c r="C78" t="s">
+        <v>228</v>
+      </c>
+      <c r="D78" t="s">
         <v>229</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>230</v>
       </c>
-      <c r="E78" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2701,16 +2899,16 @@
         <v>231</v>
       </c>
       <c r="C79" t="s">
+        <v>375</v>
+      </c>
+      <c r="D79" t="s">
         <v>232</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>233</v>
       </c>
-      <c r="E79" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2718,16 +2916,16 @@
         <v>234</v>
       </c>
       <c r="C80" t="s">
+        <v>376</v>
+      </c>
+      <c r="D80" t="s">
         <v>235</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>236</v>
       </c>
-      <c r="E80" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2735,16 +2933,16 @@
         <v>237</v>
       </c>
       <c r="C81" t="s">
+        <v>377</v>
+      </c>
+      <c r="D81" t="s">
         <v>238</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>239</v>
       </c>
-      <c r="E81" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2752,16 +2950,16 @@
         <v>240</v>
       </c>
       <c r="C82" t="s">
+        <v>378</v>
+      </c>
+      <c r="D82" t="s">
         <v>241</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>242</v>
       </c>
-      <c r="E82" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2769,16 +2967,16 @@
         <v>243</v>
       </c>
       <c r="C83" t="s">
+        <v>379</v>
+      </c>
+      <c r="D83" t="s">
         <v>244</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>245</v>
       </c>
-      <c r="E83" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2786,16 +2984,16 @@
         <v>246</v>
       </c>
       <c r="C84" t="s">
+        <v>380</v>
+      </c>
+      <c r="D84" t="s">
         <v>247</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>248</v>
       </c>
-      <c r="E84" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2803,33 +3001,33 @@
         <v>249</v>
       </c>
       <c r="C85" t="s">
+        <v>381</v>
+      </c>
+      <c r="D85" t="s">
         <v>250</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>251</v>
       </c>
-      <c r="E85" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>252</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D86" t="s">
         <v>253</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>254</v>
       </c>
-      <c r="E86" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2837,50 +3035,50 @@
         <v>255</v>
       </c>
       <c r="C87" t="s">
+        <v>383</v>
+      </c>
+      <c r="D87" t="s">
         <v>256</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>257</v>
       </c>
-      <c r="E87" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>258</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D88" t="s">
         <v>259</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>260</v>
       </c>
-      <c r="E88" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>261</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D89" t="s">
         <v>262</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>263</v>
       </c>
-      <c r="E89" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2888,16 +3086,16 @@
         <v>264</v>
       </c>
       <c r="C90" t="s">
+        <v>386</v>
+      </c>
+      <c r="D90" t="s">
         <v>265</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>266</v>
       </c>
-      <c r="E90" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2905,16 +3103,16 @@
         <v>267</v>
       </c>
       <c r="C91" t="s">
+        <v>387</v>
+      </c>
+      <c r="D91" t="s">
         <v>268</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>269</v>
       </c>
-      <c r="E91" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2922,16 +3120,16 @@
         <v>270</v>
       </c>
       <c r="C92" t="s">
+        <v>388</v>
+      </c>
+      <c r="D92" t="s">
         <v>271</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>272</v>
       </c>
-      <c r="E92" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2939,16 +3137,16 @@
         <v>273</v>
       </c>
       <c r="C93" t="s">
+        <v>389</v>
+      </c>
+      <c r="D93" t="s">
         <v>274</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>275</v>
       </c>
-      <c r="E93" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2956,16 +3154,16 @@
         <v>276</v>
       </c>
       <c r="C94" t="s">
+        <v>390</v>
+      </c>
+      <c r="D94" t="s">
         <v>277</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>278</v>
       </c>
-      <c r="E94" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2973,16 +3171,16 @@
         <v>279</v>
       </c>
       <c r="C95" t="s">
+        <v>391</v>
+      </c>
+      <c r="D95" t="s">
         <v>280</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>281</v>
       </c>
-      <c r="E95" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2990,16 +3188,16 @@
         <v>282</v>
       </c>
       <c r="C96" t="s">
+        <v>392</v>
+      </c>
+      <c r="D96" t="s">
         <v>283</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>284</v>
       </c>
-      <c r="E96" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3007,50 +3205,50 @@
         <v>285</v>
       </c>
       <c r="C97" t="s">
+        <v>285</v>
+      </c>
+      <c r="D97" t="s">
         <v>286</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>287</v>
       </c>
-      <c r="E97" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>288</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D98" t="s">
         <v>289</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>290</v>
       </c>
-      <c r="E98" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>291</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D99" t="s">
         <v>292</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>293</v>
       </c>
-      <c r="E99" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3058,16 +3256,16 @@
         <v>294</v>
       </c>
       <c r="C100" t="s">
+        <v>395</v>
+      </c>
+      <c r="D100" t="s">
         <v>295</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>296</v>
       </c>
-      <c r="E100" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3075,13 +3273,13 @@
         <v>297</v>
       </c>
       <c r="C101" t="s">
+        <v>396</v>
+      </c>
+      <c r="D101" t="s">
         <v>298</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>299</v>
-      </c>
-      <c r="E101" t="s">
-        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>